<commit_message>
Trabalho em banco de dados de materiais usados
</commit_message>
<xml_diff>
--- a/projetoLista.xlsx
+++ b/projetoLista.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="96">
   <si>
     <t>DESCRIÇÃO DECISAO</t>
   </si>
@@ -235,6 +235,78 @@
   </si>
   <si>
     <t>CONVENTO'S</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>BALANCEADOR PISADOR</t>
+  </si>
+  <si>
+    <t>BALANCEADOR</t>
+  </si>
+  <si>
+    <t>EMPURRADOR RÉGUAS /LEV</t>
+  </si>
+  <si>
+    <t>EMPURRADOR</t>
+  </si>
+  <si>
+    <t>PORTA PUNÇÃO 1020</t>
+  </si>
+  <si>
+    <t>PORTA PUNÇÃO</t>
+  </si>
+  <si>
+    <t>PORTA MATRIZ</t>
+  </si>
+  <si>
+    <t>PORTA PUNÇÃO ARTICULADO</t>
+  </si>
+  <si>
+    <t>PORTA MATRIZ DURO</t>
+  </si>
+  <si>
+    <t>COLUNA GUIA</t>
+  </si>
+  <si>
+    <t>COLUNA GUIA EXTERNA 4140</t>
+  </si>
+  <si>
+    <t>COLUNA GUIA EXTERNA 8620</t>
+  </si>
+  <si>
+    <t>COLUNA RÉGUAS</t>
+  </si>
+  <si>
+    <t>COLUNA RÉGUA</t>
+  </si>
+  <si>
+    <t>PUNÇÃO CORTE</t>
+  </si>
+  <si>
+    <t>PUNÇÃO DOBRA</t>
+  </si>
+  <si>
+    <t>PUNÇÃO FORMA</t>
+  </si>
+  <si>
+    <t>TUBO SCHED. LIMITADOR</t>
+  </si>
+  <si>
+    <t>TUBO LIMITADOR</t>
+  </si>
+  <si>
+    <t>TUBO LIMITADOR COMPLETO</t>
+  </si>
+  <si>
+    <t>LIMITADOR DE CURSO</t>
+  </si>
+  <si>
+    <t>ARRUELA TUBO LIMITADOR</t>
+  </si>
+  <si>
+    <t>SCHEDULE 80-S</t>
   </si>
 </sst>
 </file>
@@ -771,21 +843,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.7109375" customWidth="1"/>
     <col min="2" max="2" width="29.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" customWidth="1"/>
-    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="3" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" customWidth="1"/>
     <col min="6" max="6" width="13.85546875" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
   </cols>
   <sheetData>
@@ -958,219 +1029,439 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="C9" t="s">
         <v>25</v>
       </c>
-      <c r="D9" t="s">
-        <v>57</v>
+      <c r="G9" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>80</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>78</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" t="s">
-        <v>57</v>
-      </c>
-      <c r="G10" t="s">
-        <v>36</v>
+        <v>29</v>
+      </c>
+      <c r="E10" t="str">
+        <f>$H$4</f>
+        <v>T.R 54-56 Hrc</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>79</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>79</v>
       </c>
       <c r="C11" t="s">
         <v>25</v>
       </c>
-      <c r="D11" t="s">
-        <v>26</v>
-      </c>
-      <c r="G11" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>81</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>79</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="E12" t="str">
+        <f>$H$4</f>
+        <v>T.R 54-56 Hrc</v>
       </c>
       <c r="G12" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="C13" t="s">
         <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="G13" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>24</v>
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
       </c>
       <c r="C14" t="s">
         <v>25</v>
       </c>
       <c r="D14" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" t="s">
         <v>26</v>
       </c>
-      <c r="G14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="G15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>62</v>
+        <v>22</v>
+      </c>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" t="s">
+        <v>26</v>
       </c>
       <c r="G16" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>62</v>
+        <v>23</v>
+      </c>
+      <c r="C17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" t="s">
+        <v>26</v>
       </c>
       <c r="G17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="B18" t="s">
-        <v>62</v>
+        <v>74</v>
+      </c>
+      <c r="C18" t="s">
+        <v>25</v>
       </c>
       <c r="G18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="B19" t="s">
-        <v>62</v>
+        <v>76</v>
+      </c>
+      <c r="C19" t="s">
+        <v>25</v>
       </c>
       <c r="G19" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="B20" t="s">
-        <v>70</v>
+        <v>91</v>
+      </c>
+      <c r="C20" t="s">
+        <v>95</v>
       </c>
       <c r="G20" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>67</v>
+        <v>92</v>
       </c>
       <c r="B21" t="s">
-        <v>70</v>
+        <v>93</v>
+      </c>
+      <c r="C21" t="s">
+        <v>25</v>
       </c>
       <c r="G21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>68</v>
-      </c>
-      <c r="B22" t="s">
-        <v>70</v>
+        <v>94</v>
+      </c>
+      <c r="C22" t="s">
+        <v>25</v>
       </c>
       <c r="G22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>84</v>
+      </c>
+      <c r="B23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" t="str">
+        <f>$H$7</f>
+        <v>C.T.R 60-62 Hrc</v>
+      </c>
+      <c r="G23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>83</v>
+      </c>
+      <c r="B24" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" t="str">
+        <f>$H$7</f>
+        <v>C.T.R 60-62 Hrc</v>
+      </c>
+      <c r="G24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>85</v>
+      </c>
+      <c r="B25" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" t="s">
+        <v>36</v>
+      </c>
+      <c r="G25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>87</v>
+      </c>
+      <c r="B26" t="s">
+        <v>87</v>
+      </c>
+      <c r="C26" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26" t="str">
+        <f>$H$6</f>
+        <v>T.R 60-62 Hrc</v>
+      </c>
+      <c r="G26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" t="s">
+        <v>88</v>
+      </c>
+      <c r="C27" t="s">
+        <v>30</v>
+      </c>
+      <c r="E27" t="str">
+        <f>$H$6</f>
+        <v>T.R 60-62 Hrc</v>
+      </c>
+      <c r="G27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>89</v>
+      </c>
+      <c r="B28" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28" t="s">
+        <v>30</v>
+      </c>
+      <c r="E28" t="str">
+        <f>$H$6</f>
+        <v>T.R 60-62 Hrc</v>
+      </c>
+      <c r="G28" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" t="s">
+        <v>26</v>
+      </c>
+      <c r="G29" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G30">
+        <v>1.2768999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" t="str">
+        <f>$G$22</f>
+        <v>PRODTY</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" t="str">
+        <f>$G$23</f>
+        <v>KALLER</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" t="str">
+        <f>$G$25</f>
+        <v>AZOL GAS</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" t="str">
+        <f>$G$24</f>
+        <v>DADCO</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" t="str">
+        <f>$G$22</f>
+        <v>PRODTY</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>67</v>
+      </c>
+      <c r="B36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C36" t="str">
+        <f>$G$23</f>
+        <v>KALLER</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37" t="s">
+        <v>70</v>
+      </c>
+      <c r="C37" t="str">
+        <f>$G$25</f>
+        <v>AZOL GAS</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>69</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B38" t="s">
         <v>70</v>
       </c>
-      <c r="G23" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G24" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G26" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G27" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G28">
-        <v>1.2768999999999999</v>
+      <c r="C38" t="str">
+        <f>$G$24</f>
+        <v>DADCO</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>